<commit_message>
Update PubMed class to filter for affiliation
</commit_message>
<xml_diff>
--- a/example_input.xlsx
+++ b/example_input.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JLH7459/publication-scraper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbeavers/Documents/GitHub/publication-scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD5904CD-C976-5F4B-8ACF-959B8C3062D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A30A5E-5464-824A-822F-5D4CD0989011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{D894F065-5AA2-3F42-93CB-4D37D05B9DC2}"/>
+    <workbookView xWindow="2280" yWindow="980" windowWidth="27640" windowHeight="16940" xr2:uid="{D894F065-5AA2-3F42-93CB-4D37D05B9DC2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="utrc_active_allocations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>root_institution_name</t>
   </si>
@@ -47,44 +47,35 @@
     <t>last_name</t>
   </si>
   <si>
-    <t>The University of Texas</t>
-  </si>
-  <si>
-    <t>Tejna</t>
-  </si>
-  <si>
-    <t>Dasari</t>
-  </si>
-  <si>
     <t>The University of Texas at Austin</t>
   </si>
   <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Urban</t>
-  </si>
-  <si>
-    <t>lee</t>
-  </si>
-  <si>
-    <t>xiaolong</t>
-  </si>
-  <si>
-    <t>The University of Texas at San Antonio</t>
-  </si>
-  <si>
-    <t>Sanjeeth</t>
-  </si>
-  <si>
-    <t>Boddinagula</t>
+    <t>Beavers</t>
+  </si>
+  <si>
+    <t>Kelsey m</t>
+  </si>
+  <si>
+    <t>Carson</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Mydlarz</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>The University of Texas at Arlington</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -95,8 +86,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,9 +117,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,67 +455,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FF3394-87E0-7B40-9D31-5BE749F425B0}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="A5" sqref="A5:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>